<commit_message>
RTM updates and Youtrack bug sheet
</commit_message>
<xml_diff>
--- a/Documentation/RTM/RTM.xlsx
+++ b/Documentation/RTM/RTM.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>PROJECT INFORMATION</t>
   </si>
@@ -72,6 +72,36 @@
   </si>
   <si>
     <t>Test Case Ref</t>
+  </si>
+  <si>
+    <t>https://github.com/sangeetajoshi/E-Appointment_Final/tree/master/Documentation/SRS</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>Make Appointment Prospect Student</t>
+  </si>
+  <si>
+    <t>Make Appointment Current  Student</t>
+  </si>
+  <si>
+    <t>View Appointment - Faculty/Student</t>
+  </si>
+  <si>
+    <t>Set Up Appointment</t>
+  </si>
+  <si>
+    <t>Admin- Ad/Update/Delete User</t>
+  </si>
+  <si>
+    <t>Edit Profile(Change Password)</t>
+  </si>
+  <si>
+    <t>Sign Out</t>
+  </si>
+  <si>
+    <t>https://github.com/sangeetajoshi/E-Appointment_Final/tree/master/Testing/Test%20Cases</t>
   </si>
 </sst>
 </file>
@@ -122,7 +152,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -265,13 +295,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
       <protection locked="0"/>
@@ -293,25 +344,16 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -641,65 +683,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="42" style="10" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="40.83203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="5" spans="1:5" ht="29" customHeight="1">
-      <c r="A5" s="6" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="5" spans="1:5" ht="20" customHeight="1">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="11" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45">
+      <c r="A13" s="1">
+        <v>8</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RTM source code location updated
</commit_message>
<xml_diff>
--- a/Documentation/RTM/RTM.xlsx
+++ b/Documentation/RTM/RTM.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t>PROJECT INFORMATION</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>https://github.com/sangeetajoshi/E-Appointment_Final/tree/master/Testing/Test%20Cases</t>
+  </si>
+  <si>
+    <t>https://github.com/sangeetajoshi/E-Appointment_Final/tree/master/Source%20Code/EAppointment</t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -305,8 +308,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -314,6 +318,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -341,11 +348,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -354,6 +361,7 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -685,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -700,47 +708,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -754,6 +762,9 @@
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D6" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
@@ -768,6 +779,9 @@
       <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
@@ -782,6 +796,9 @@
       <c r="C8" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D8" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
@@ -796,6 +813,9 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D9" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
@@ -810,6 +830,9 @@
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D10" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
       </c>
@@ -824,6 +847,9 @@
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D11" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
       </c>
@@ -838,6 +864,9 @@
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D12" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
@@ -851,6 +880,9 @@
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
@@ -862,9 +894,19 @@
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D8" r:id="rId3"/>
+    <hyperlink ref="D9" r:id="rId4"/>
+    <hyperlink ref="D10" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
+    <hyperlink ref="D12" r:id="rId7"/>
+    <hyperlink ref="D13" r:id="rId8"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId9"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>